<commit_message>
Modifikasi Template Kategori EXCEL (UTS)
</commit_message>
<xml_diff>
--- a/public/template_kategori.xlsx
+++ b/public/template_kategori.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Semester_4\PemrogramanWeb\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F61E6D75-5BCE-455E-80D7-5F86E8BE8CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE01DD32-8A8A-4944-805B-DE3244D68A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{309343A3-4143-4EFE-810F-12D7ABF4FBBA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{309343A3-4143-4EFE-810F-12D7ABF4FBBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>kategori_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>kategori_kode</t>
   </si>
@@ -421,61 +418,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACA0E51-3E30-4508-BE2C-BB0CF361000A}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>